<commit_message>
Realizar reunion diaria (daily meeting)
</commit_message>
<xml_diff>
--- a/Desarrollo/SGPI/Sprint 02/0 Gestion de proyectos/SGPI_PB.xlsx
+++ b/Desarrollo/SGPI/Sprint 02/0 Gestion de proyectos/SGPI_PB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Escritorio\Maestrias\MII\CICLO 04\Gestion de la confirguracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\maestria\ciclo IV\gestion configuracion\Repositorio\GCS-JWD\Desarrollo\SGPI\Sprint 02\0 Gestion de proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D469D2D-C6CF-4386-9C29-A422D1BFCDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012EEE34-411D-494B-AC63-C54692272F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Untitled query" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -158,12 +158,24 @@
   </si>
   <si>
     <t>Retrospectiva del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -997,16 +1009,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>73</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>74</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>75</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>76</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>77</v>
       </c>
@@ -1120,7 +1132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>78</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>79</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>56</v>
       </c>
@@ -1170,8 +1182,11 @@
       <c r="G9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>57</v>
       </c>
@@ -1190,8 +1205,11 @@
       <c r="G10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>58</v>
       </c>
@@ -1210,8 +1228,11 @@
       <c r="G11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>59</v>
       </c>
@@ -1228,7 +1249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>61</v>
       </c>
@@ -1248,7 +1269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>62</v>
       </c>
@@ -1264,8 +1285,11 @@
       <c r="G14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>63</v>
       </c>
@@ -1282,7 +1306,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>64</v>
       </c>
@@ -1299,7 +1323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>60</v>
       </c>
@@ -1316,7 +1340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>65</v>
       </c>
@@ -1332,8 +1356,11 @@
       <c r="G18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>66</v>
       </c>
@@ -1350,7 +1377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>67</v>
       </c>
@@ -1366,8 +1393,11 @@
       <c r="G20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>68</v>
       </c>
@@ -1384,7 +1414,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>69</v>
       </c>
@@ -1401,7 +1431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>70</v>
       </c>
@@ -1417,8 +1447,11 @@
       <c r="G23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>71</v>
       </c>
@@ -1435,7 +1468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>72</v>
       </c>
@@ -1452,7 +1485,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>80</v>
       </c>
@@ -1469,7 +1502,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>81</v>
       </c>
@@ -1486,7 +1519,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>82</v>
       </c>

</xml_diff>